<commit_message>
Extended excel reading examples
</commit_message>
<xml_diff>
--- a/chapter20/sample.xlsx
+++ b/chapter20/sample.xlsx
@@ -1,39 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeh/PycharmProjects/advancedpython3/chapter20/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B79977-C615-C54D-80DD-761740F8FF27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="my worksheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="my other sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="my worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="my other sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phoebe </t>
+  </si>
+  <si>
+    <t>Gryff</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>Gingy</t>
+  </si>
+  <si>
+    <t>Joppa</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,15 +91,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -345,75 +396,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor rgb="001072BA"/>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <tabColor rgb="FF1072BA"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>21</v>
+      </c>
+      <c r="C1">
+        <v>56</v>
+      </c>
+      <c r="D1">
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <f>(C1+D1)/2</f>
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <f>SUM(A1, A2)</f>
-        <v/>
+      <c r="D2">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E9" si="0">(C2+D2)/2</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>55</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>67</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>67</v>
+      </c>
+      <c r="D7">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>87</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>45.5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
         <v>3.42</v>
       </c>
-      <c r="B1" t="n">
+      <c r="B1">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>